<commit_message>
feat: add styles, delete second json file
</commit_message>
<xml_diff>
--- a/queue/info/данные/новые/ТЭТС.xlsx
+++ b/queue/info/данные/новые/ТЭТС.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Disk\WEB\CV\queue\info\данные\новые\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B74C278-1FC7-48D8-A207-AAB309DE0E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD308F61-D9AF-48F0-B22A-EC11FA080C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2760" yWindow="4275" windowWidth="18495" windowHeight="8400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ГОКБ" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11353" uniqueCount="5063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11355" uniqueCount="5063">
   <si>
     <t>№ п.п.</t>
   </si>
@@ -16480,14 +16480,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -18022,8 +18022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A6491F-9941-4642-9B58-151C15BAD05D}">
   <dimension ref="A1:K447"/>
   <sheetViews>
-    <sheetView topLeftCell="A230" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268:XFD268"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22574,7 +22574,9 @@
         <v>15</v>
       </c>
       <c r="I144" s="160"/>
-      <c r="J144" s="156"/>
+      <c r="J144" s="156" t="s">
+        <v>5056</v>
+      </c>
       <c r="K144" s="157" t="s">
         <v>335</v>
       </c>
@@ -22605,7 +22607,9 @@
         <v>15</v>
       </c>
       <c r="I145" s="126"/>
-      <c r="J145" s="133"/>
+      <c r="J145" s="133" t="s">
+        <v>5056</v>
+      </c>
       <c r="K145" s="140" t="s">
         <v>338</v>
       </c>
@@ -31666,8 +31670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q1062"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31678,10 +31682,10 @@
     <col min="4" max="4" width="7.7109375" style="81" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="81" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" style="81" customWidth="1"/>
-    <col min="7" max="7" width="59.42578125" style="82" customWidth="1"/>
+    <col min="7" max="7" width="49.85546875" style="82" customWidth="1"/>
     <col min="8" max="8" width="18.140625" style="81" customWidth="1"/>
     <col min="9" max="10" width="12.42578125" style="81" customWidth="1"/>
-    <col min="11" max="11" width="42.7109375" style="81" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" style="81" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" style="81" customWidth="1"/>
     <col min="13" max="13" width="30.28515625" style="81" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" style="81" customWidth="1"/>
@@ -31725,7 +31729,7 @@
       <c r="L1" s="97" t="s">
         <v>910</v>
       </c>
-      <c r="M1" s="199" t="s">
+      <c r="M1" s="197" t="s">
         <v>9</v>
       </c>
       <c r="N1" s="97" t="s">
@@ -33845,7 +33849,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="85">
         <v>4138</v>
       </c>
@@ -34169,7 +34173,7 @@
       <c r="K69" s="100"/>
       <c r="L69" s="92"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="92">
         <v>4147</v>
       </c>
@@ -34737,7 +34741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="85">
         <v>4162</v>
       </c>
@@ -35429,7 +35433,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="88">
         <v>4180</v>
       </c>
@@ -35747,7 +35751,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="85">
         <v>4189</v>
       </c>
@@ -36271,7 +36275,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="85">
         <v>4204</v>
       </c>
@@ -36446,7 +36450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="85">
         <v>4209</v>
       </c>
@@ -38531,7 +38535,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="85">
         <v>4265</v>
       </c>
@@ -39022,7 +39026,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="85">
         <v>4279</v>
       </c>
@@ -39124,7 +39128,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="85">
         <v>4282</v>
       </c>
@@ -39792,7 +39796,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="85">
         <v>4300</v>
       </c>
@@ -43587,7 +43591,7 @@
       </c>
       <c r="M325" s="94"/>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A326" s="85">
         <v>4403</v>
       </c>
@@ -45370,7 +45374,7 @@
       </c>
       <c r="N372" s="88"/>
     </row>
-    <row r="373" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A373" s="85">
         <v>4450</v>
       </c>
@@ -45983,7 +45987,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="389" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A389" s="85">
         <v>4466</v>
       </c>
@@ -47392,7 +47396,7 @@
       </c>
       <c r="N429" s="88"/>
     </row>
-    <row r="430" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A430" s="85">
         <v>4507</v>
       </c>
@@ -48936,7 +48940,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="474" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A474" s="85">
         <v>4551</v>
       </c>
@@ -48970,7 +48974,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="475" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A475" s="85">
         <v>4552</v>
       </c>
@@ -50412,7 +50416,7 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="527" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A527" s="85">
         <v>4604</v>
       </c>
@@ -51443,7 +51447,7 @@
       </c>
       <c r="Q564" s="88"/>
     </row>
-    <row r="565" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A565" s="88">
         <v>4642</v>
       </c>
@@ -52353,7 +52357,7 @@
       <c r="O594" s="88"/>
       <c r="P594" s="88"/>
     </row>
-    <row r="595" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A595" s="88">
         <v>4672</v>
       </c>
@@ -52585,7 +52589,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="603" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A603" s="88">
         <v>4680</v>
       </c>
@@ -53358,7 +53362,7 @@
         <v>2595</v>
       </c>
     </row>
-    <row r="630" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="630" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A630" s="85">
         <v>4707</v>
       </c>
@@ -53550,7 +53554,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="637" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="637" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A637" s="88">
         <v>4714</v>
       </c>
@@ -53700,7 +53704,7 @@
         <v>2627</v>
       </c>
     </row>
-    <row r="642" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A642" s="85">
         <v>4719</v>
       </c>
@@ -53752,7 +53756,7 @@
         <v>2633</v>
       </c>
     </row>
-    <row r="644" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A644" s="85">
         <v>4721</v>
       </c>
@@ -53970,7 +53974,7 @@
       <c r="O651" s="103"/>
       <c r="P651" s="103"/>
     </row>
-    <row r="652" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A652" s="103">
         <v>4729</v>
       </c>
@@ -56827,7 +56831,7 @@
         <v>2946</v>
       </c>
     </row>
-    <row r="757" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="757" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A757" s="85">
         <v>4834</v>
       </c>
@@ -57696,7 +57700,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="789" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="789" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A789" s="85">
         <v>4866</v>
       </c>
@@ -59504,7 +59508,7 @@
         <v>3214</v>
       </c>
     </row>
-    <row r="854" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="854" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A854" s="85">
         <v>4931</v>
       </c>
@@ -60016,7 +60020,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="874" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="874" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A874" s="85">
         <v>4951</v>
       </c>
@@ -62078,7 +62082,7 @@
         <v>3471</v>
       </c>
     </row>
-    <row r="953" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="953" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A953" s="85">
         <v>5030</v>
       </c>
@@ -63705,7 +63709,7 @@
       <c r="M1008" s="117"/>
       <c r="N1008" s="117"/>
     </row>
-    <row r="1009" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1009" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A1009" s="117">
         <v>5086</v>
       </c>
@@ -64091,7 +64095,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1022" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1022" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A1022" s="85">
         <v>5099</v>
       </c>
@@ -64143,7 +64147,7 @@
         <v>2092</v>
       </c>
     </row>
-    <row r="1024" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1024" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A1024" s="85">
         <v>5101</v>
       </c>
@@ -65163,7 +65167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -65248,11 +65252,11 @@
       <c r="K2" s="67" t="s">
         <v>3756</v>
       </c>
-      <c r="L2" s="197"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
-      <c r="P2" s="198"/>
+      <c r="L2" s="198"/>
+      <c r="M2" s="199"/>
+      <c r="N2" s="199"/>
+      <c r="O2" s="199"/>
+      <c r="P2" s="199"/>
     </row>
     <row r="3" spans="1:16" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="63">

</xml_diff>